<commit_message>
updated medium severity to critical
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/Autochek_Address_Modification_Negative-api-data.xlsx
+++ b/src/test/java/TestData/Autochek_Address_Modification_Negative-api-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satti\Testing\Autochek\github\autocheck-api-automation\src\test\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satti\Testing\Autochek\github\autochek-api-automation\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B847430-AAA5-4C6C-BF6B-C2AA5777398C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1EB218-A90D-4F6D-AB68-3E613E0CF7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4032" yWindow="3144" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Get Franchise Negative" sheetId="1" r:id="rId1"/>
@@ -3453,7 +3453,7 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -3559,7 +3559,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>561</v>
+        <v>8</v>
       </c>
       <c r="C5" s="59" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
updated the severity back to medium
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/Autochek_Address_Modification_Negative-api-data.xlsx
+++ b/src/test/java/TestData/Autochek_Address_Modification_Negative-api-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satti\Testing\Autochek\github\autochek-api-automation\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1EB218-A90D-4F6D-AB68-3E613E0CF7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2960735C-E45F-4D03-8E76-95404E8180D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4032" yWindow="3144" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Get Franchise Negative" sheetId="1" r:id="rId1"/>
@@ -3559,7 +3559,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>8</v>
+        <v>561</v>
       </c>
       <c r="C5" s="59" t="s">
         <v>14</v>

</xml_diff>